<commit_message>
Updating excel in Duplicate branch
Commiting excel in Duplicate branch
</commit_message>
<xml_diff>
--- a/Excel1.xlsx
+++ b/Excel1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,12 +331,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>